<commit_message>
Try branch add 1
</commit_message>
<xml_diff>
--- a/LU/Test_results_LUDecomposition.xlsx
+++ b/LU/Test_results_LUDecomposition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuan &amp; Yi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuan &amp; Yi\Desktop\TestingProgram\LU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -938,7 +938,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -949,7 +949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -960,7 +960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -971,7 +971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -981,8 +981,11 @@
       <c r="C20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>